<commit_message>
updated up to Dec-05 release
</commit_message>
<xml_diff>
--- a/00-UAT/PROD-Release/00-ALL Releases.xlsx
+++ b/00-UAT/PROD-Release/00-ALL Releases.xlsx
@@ -8,29 +8,31 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\bfl.local\dfsroot\US_Users\duque\My Documents\00-MyDocuments\00-UAT\PROD-Release\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D4EC787-D0C1-484C-9820-E28793DDD6DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60B8030E-AE3F-4756-AF70-58B5BFFE8DCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5580" yWindow="15" windowWidth="22110" windowHeight="7800" activeTab="1" xr2:uid="{71C45C7C-5B6B-4D11-BBC8-25501E7D8CDC}"/>
+    <workbookView xWindow="8295" yWindow="3885" windowWidth="19035" windowHeight="11130" activeTab="1" xr2:uid="{71C45C7C-5B6B-4D11-BBC8-25501E7D8CDC}"/>
   </bookViews>
   <sheets>
     <sheet name="General Check list" sheetId="2" r:id="rId1"/>
-    <sheet name="Prod-Nov-23-2022" sheetId="18" r:id="rId2"/>
-    <sheet name="Prod-Nov-11-2022" sheetId="17" r:id="rId3"/>
-    <sheet name="Prod-Nov-04-2022" sheetId="16" r:id="rId4"/>
-    <sheet name="Prod-Oct-21-2022" sheetId="15" r:id="rId5"/>
-    <sheet name="Prod-Oct-14-2022" sheetId="14" r:id="rId6"/>
-    <sheet name="Prod-Oct-07-2022" sheetId="11" r:id="rId7"/>
-    <sheet name="Sep Successes" sheetId="13" r:id="rId8"/>
-    <sheet name="Prod-Sep-29-2022" sheetId="12" r:id="rId9"/>
-    <sheet name="Prod-Sep-16-2022" sheetId="10" r:id="rId10"/>
-    <sheet name="Prod-Sep-09-2022" sheetId="8" r:id="rId11"/>
-    <sheet name="Aug Successes" sheetId="9" r:id="rId12"/>
-    <sheet name="Prod-Aug-26-Sep-12022" sheetId="7" r:id="rId13"/>
-    <sheet name="Prod-Aug-12-2022" sheetId="6" r:id="rId14"/>
-    <sheet name="Prod-Aug-05-2022" sheetId="5" r:id="rId15"/>
-    <sheet name="Prod-July-22-2022" sheetId="4" r:id="rId16"/>
-    <sheet name="Prod-July-15-2022" sheetId="3" r:id="rId17"/>
-    <sheet name="Prod-July-1-2022" sheetId="1" r:id="rId18"/>
+    <sheet name="Prod-Dec-05-2022" sheetId="20" r:id="rId2"/>
+    <sheet name="Prod-Nov-28-2022" sheetId="19" r:id="rId3"/>
+    <sheet name="Prod-Nov-23-2022" sheetId="18" r:id="rId4"/>
+    <sheet name="Prod-Nov-11-2022" sheetId="17" r:id="rId5"/>
+    <sheet name="Prod-Nov-04-2022" sheetId="16" r:id="rId6"/>
+    <sheet name="Prod-Oct-21-2022" sheetId="15" r:id="rId7"/>
+    <sheet name="Prod-Oct-14-2022" sheetId="14" r:id="rId8"/>
+    <sheet name="Prod-Oct-07-2022" sheetId="11" r:id="rId9"/>
+    <sheet name="Sep Successes" sheetId="13" r:id="rId10"/>
+    <sheet name="Prod-Sep-29-2022" sheetId="12" r:id="rId11"/>
+    <sheet name="Prod-Sep-16-2022" sheetId="10" r:id="rId12"/>
+    <sheet name="Prod-Sep-09-2022" sheetId="8" r:id="rId13"/>
+    <sheet name="Aug Successes" sheetId="9" r:id="rId14"/>
+    <sheet name="Prod-Aug-26-Sep-12022" sheetId="7" r:id="rId15"/>
+    <sheet name="Prod-Aug-12-2022" sheetId="6" r:id="rId16"/>
+    <sheet name="Prod-Aug-05-2022" sheetId="5" r:id="rId17"/>
+    <sheet name="Prod-July-22-2022" sheetId="4" r:id="rId18"/>
+    <sheet name="Prod-July-15-2022" sheetId="3" r:id="rId19"/>
+    <sheet name="Prod-July-1-2022" sheetId="1" r:id="rId20"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -52,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1152" uniqueCount="385">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1339" uniqueCount="439">
   <si>
     <t>Bugs</t>
   </si>
@@ -1272,12 +1274,174 @@
     <t>Test
 Status</t>
   </si>
+  <si>
+    <t>VG00004445AA</t>
+  </si>
+  <si>
+    <t>WG00004446AA</t>
+  </si>
+  <si>
+    <t>VG00004447AA</t>
+  </si>
+  <si>
+    <t>VG00004448AA</t>
+  </si>
+  <si>
+    <t>WG00004449AA</t>
+  </si>
+  <si>
+    <t>VG00004450AA</t>
+  </si>
+  <si>
+    <t>VG00004451AA</t>
+  </si>
+  <si>
+    <t>VG00004481AA</t>
+  </si>
+  <si>
+    <t>VG00004482AA</t>
+  </si>
+  <si>
+    <t>VG00004480AA</t>
+  </si>
+  <si>
+    <t>VG00004452AA</t>
+  </si>
+  <si>
+    <t>VG00004453AA</t>
+  </si>
+  <si>
+    <t> VG00004454AA</t>
+  </si>
+  <si>
+    <t>VG00004455AA</t>
+  </si>
+  <si>
+    <t>VG00004479AA</t>
+  </si>
+  <si>
+    <t>VG00004483AA</t>
+  </si>
+  <si>
+    <t>BBR - Update Standard SLDFs - Effective 11-29-2022</t>
+  </si>
+  <si>
+    <t>BD-12879</t>
+  </si>
+  <si>
+    <t>VG00004488AA</t>
+  </si>
+  <si>
+    <t>WG00004489AA</t>
+  </si>
+  <si>
+    <t>VG00004490AA</t>
+  </si>
+  <si>
+    <t>VG00004491AA</t>
+  </si>
+  <si>
+    <t>WG00004492AA</t>
+  </si>
+  <si>
+    <t>VG00004493AA</t>
+  </si>
+  <si>
+    <t>VG00004494AA</t>
+  </si>
+  <si>
+    <t>VG00004495AA</t>
+  </si>
+  <si>
+    <t>VG00004501AA</t>
+  </si>
+  <si>
+    <t>VG00004503AA</t>
+  </si>
+  <si>
+    <t>VG00004496AA</t>
+  </si>
+  <si>
+    <t>VG00004497AA</t>
+  </si>
+  <si>
+    <t>VG00004498AA</t>
+  </si>
+  <si>
+    <t>VG00004499AA</t>
+  </si>
+  <si>
+    <t>VG00004504AA</t>
+  </si>
+  <si>
+    <t>VG00004502AA</t>
+  </si>
+  <si>
+    <t>BMT - ASAP - Update 2023 Lloyd's Security Schedule with new 2023 wording from Compliance - Non-Admitted Effective 1/1/2023</t>
+  </si>
+  <si>
+    <t>BD-14861</t>
+  </si>
+  <si>
+    <t>BBR - ASAP - Update 2023 Lloyd's Security Schedule with new 2023 wording from Compliance - Non-Admitted Effective 1/1/2023</t>
+  </si>
+  <si>
+    <t>BD-14870</t>
+  </si>
+  <si>
+    <t>VG00004524AA</t>
+  </si>
+  <si>
+    <t>WG00004525AA</t>
+  </si>
+  <si>
+    <t>VG00004526AA</t>
+  </si>
+  <si>
+    <t>VG00004527AA</t>
+  </si>
+  <si>
+    <t>WG00004528AA</t>
+  </si>
+  <si>
+    <t>VG00004529AA</t>
+  </si>
+  <si>
+    <t>VG00004530AA</t>
+  </si>
+  <si>
+    <t>VG00004538AA</t>
+  </si>
+  <si>
+    <t>VG00004539AA</t>
+  </si>
+  <si>
+    <t>VG00004543AA</t>
+  </si>
+  <si>
+    <t>VG00004533AA</t>
+  </si>
+  <si>
+    <t>VG00004532AA</t>
+  </si>
+  <si>
+    <t>VG00004534AA</t>
+  </si>
+  <si>
+    <t>VG00004537AA</t>
+  </si>
+  <si>
+    <t>VG00004544AA</t>
+  </si>
+  <si>
+    <t>VG00004541AA</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1343,6 +1507,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1499,10 +1671,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1653,8 +1826,18 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -4439,7 +4622,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{674EFA29-22CC-457A-B62F-EECD60DEBE9F}">
   <dimension ref="A2:F82"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" workbookViewId="0">
+    <sheetView topLeftCell="D2" workbookViewId="0">
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
@@ -4708,6 +4891,441 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34226C2A-68CD-4BD9-A906-AC8705245632}">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" customWidth="1"/>
+    <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="33" t="s">
+        <v>188</v>
+      </c>
+      <c r="B1" s="34" t="s">
+        <v>189</v>
+      </c>
+      <c r="C1" s="34" t="s">
+        <v>190</v>
+      </c>
+      <c r="D1" s="34" t="s">
+        <v>191</v>
+      </c>
+      <c r="E1" s="34" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="32" t="s">
+        <v>218</v>
+      </c>
+      <c r="B2" s="32">
+        <v>1</v>
+      </c>
+      <c r="C2" s="32">
+        <v>6</v>
+      </c>
+      <c r="D2" s="32">
+        <v>0</v>
+      </c>
+      <c r="E2" s="32" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="32" t="s">
+        <v>220</v>
+      </c>
+      <c r="B3" s="32">
+        <v>1</v>
+      </c>
+      <c r="C3" s="32">
+        <v>2</v>
+      </c>
+      <c r="D3" s="32">
+        <v>0</v>
+      </c>
+      <c r="E3" s="32" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="32" t="s">
+        <v>222</v>
+      </c>
+      <c r="B4" s="32">
+        <v>1</v>
+      </c>
+      <c r="C4" s="32">
+        <v>2</v>
+      </c>
+      <c r="D4" s="32">
+        <v>0</v>
+      </c>
+      <c r="E4" s="32" t="s">
+        <v>223</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E786991-4988-4254-B35C-AD773FF122DA}">
+  <dimension ref="A1:R39"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" style="4" customWidth="1"/>
+    <col min="3" max="3" width="132.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="1"/>
+    <col min="5" max="5" width="6.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="9.140625" style="1"/>
+    <col min="8" max="8" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" style="1"/>
+    <col min="10" max="10" width="9.140625" style="4"/>
+    <col min="11" max="15" width="9.140625" style="1"/>
+    <col min="16" max="16" width="51.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.140625" style="1"/>
+    <col min="19" max="19" width="22.42578125" style="1" customWidth="1"/>
+    <col min="20" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A1" s="23"/>
+      <c r="H1" s="4"/>
+    </row>
+    <row r="2" spans="1:18" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>187</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="H2" s="15" t="s">
+        <v>200</v>
+      </c>
+      <c r="I2" s="15" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" s="30"/>
+      <c r="B3" s="11" t="s">
+        <v>206</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>205</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="37" t="s">
+        <v>217</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" s="30"/>
+      <c r="B4" s="11" t="s">
+        <v>215</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>216</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="37" t="s">
+        <v>217</v>
+      </c>
+      <c r="F4" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" s="36"/>
+      <c r="B5" s="28"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="36"/>
+      <c r="F5" s="35"/>
+      <c r="G5" s="35"/>
+      <c r="H5" s="35"/>
+      <c r="I5" s="35"/>
+      <c r="O5" s="4"/>
+      <c r="P5" s="4"/>
+      <c r="Q5" s="4"/>
+      <c r="R5" s="4"/>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6" s="36"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="35"/>
+      <c r="H6" s="35"/>
+      <c r="I6" s="35"/>
+      <c r="O6" s="4"/>
+      <c r="P6" s="4"/>
+      <c r="Q6" s="4"/>
+      <c r="R6" s="4"/>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="5"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+    </row>
+    <row r="11" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="J11" s="4"/>
+    </row>
+    <row r="12" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="J12" s="4"/>
+    </row>
+    <row r="13" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="J13" s="4"/>
+    </row>
+    <row r="14" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="B14" s="5"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="J14" s="4"/>
+    </row>
+    <row r="15" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="J15" s="4"/>
+    </row>
+    <row r="16" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="J16" s="4"/>
+    </row>
+    <row r="17" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="J17" s="4"/>
+    </row>
+    <row r="18" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="J18" s="4"/>
+    </row>
+    <row r="19" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="J19" s="4"/>
+    </row>
+    <row r="20" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="J20" s="4"/>
+    </row>
+    <row r="21" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D21" s="1"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="J21" s="4"/>
+    </row>
+    <row r="22" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="30"/>
+      <c r="B22" s="11" t="s">
+        <v>206</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>205</v>
+      </c>
+      <c r="D22" s="1"/>
+      <c r="E22" s="4"/>
+      <c r="J22" s="4"/>
+    </row>
+    <row r="23" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="30"/>
+      <c r="B23" s="11" t="s">
+        <v>215</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>216</v>
+      </c>
+      <c r="E23" s="4"/>
+      <c r="J23" s="4"/>
+    </row>
+    <row r="24" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="J24" s="4"/>
+    </row>
+    <row r="25" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="J25" s="4"/>
+    </row>
+    <row r="26" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="J26" s="4"/>
+    </row>
+    <row r="27" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="J27" s="4"/>
+    </row>
+    <row r="28" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="J28" s="4"/>
+    </row>
+    <row r="29" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="J29" s="4"/>
+    </row>
+    <row r="30" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="J30" s="4"/>
+    </row>
+    <row r="31" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="4"/>
+      <c r="E31" s="4"/>
+      <c r="J31" s="4"/>
+    </row>
+    <row r="32" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="4"/>
+      <c r="E32" s="4"/>
+      <c r="J32" s="4"/>
+    </row>
+    <row r="33" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="4"/>
+      <c r="E33" s="4"/>
+      <c r="J33" s="4"/>
+    </row>
+    <row r="34" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="4"/>
+      <c r="E34" s="4"/>
+      <c r="J34" s="4"/>
+    </row>
+    <row r="35" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="4"/>
+      <c r="E35" s="4"/>
+      <c r="J35" s="4"/>
+    </row>
+    <row r="36" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="4"/>
+      <c r="E36" s="4"/>
+      <c r="J36" s="4"/>
+    </row>
+    <row r="37" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="4"/>
+      <c r="E37" s="4"/>
+      <c r="J37" s="4"/>
+    </row>
+    <row r="38" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="4"/>
+      <c r="E38" s="4"/>
+      <c r="J38" s="4"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" s="3"/>
+      <c r="C39" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27701F9E-3FD9-4A42-BDE1-741BAA025556}">
   <dimension ref="A1:R39"/>
   <sheetViews>
@@ -5060,7 +5678,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2D62123-6C5C-409D-AECB-24FB133D4F50}">
   <dimension ref="A1:R45"/>
   <sheetViews>
@@ -5527,7 +6145,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC8F2BBC-7E6A-4493-88B1-84CDCC47D51A}">
   <dimension ref="A1:E4"/>
   <sheetViews>
@@ -5617,7 +6235,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30CBEE1B-E4A9-4E10-BBCD-608FC68D2FD8}">
   <dimension ref="A1:R47"/>
   <sheetViews>
@@ -6109,7 +6727,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1833B11-57E5-4E5E-9A84-D0565298A823}">
   <dimension ref="A1:R46"/>
   <sheetViews>
@@ -6492,7 +7110,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0B628DA-6489-4BCA-BD3F-0DBC11824F3F}">
   <dimension ref="A1:R51"/>
   <sheetViews>
@@ -6988,7 +7606,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D728167-C1FD-49BB-9BF5-602B66CE6497}">
   <dimension ref="A1:R53"/>
   <sheetViews>
@@ -7525,7 +8143,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{998DBAF6-1AA9-4799-8D61-667BEE060E7B}">
   <dimension ref="A1:P56"/>
   <sheetViews>
@@ -7997,7 +8615,574 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F26B94A-5F23-4513-A446-E4C4A9781140}">
+  <dimension ref="A1:Q53"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C31" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="M52" sqref="M52"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" style="4" customWidth="1"/>
+    <col min="3" max="3" width="127.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="1"/>
+    <col min="5" max="5" width="6.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="9.140625" style="1"/>
+    <col min="8" max="8" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" style="1"/>
+    <col min="10" max="10" width="9.140625" style="4"/>
+    <col min="11" max="11" width="9.140625" style="1"/>
+    <col min="12" max="12" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.140625" style="1"/>
+    <col min="16" max="16" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" s="23"/>
+      <c r="H1" s="4"/>
+    </row>
+    <row r="2" spans="1:17" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>187</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>384</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>200</v>
+      </c>
+      <c r="H2" s="15" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" s="30"/>
+      <c r="B3" s="11" t="s">
+        <v>420</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>419</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="37" t="s">
+        <v>333</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" s="30"/>
+      <c r="B4" s="11" t="s">
+        <v>422</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>421</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="37" t="s">
+        <v>333</v>
+      </c>
+      <c r="F4" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="H4" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="N4" s="43"/>
+      <c r="O4" s="43"/>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="4"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" s="30"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="4"/>
+      <c r="Q5" s="4"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" s="30"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="49"/>
+      <c r="N6" s="44"/>
+      <c r="O6" s="44"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" s="30"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+      <c r="N7" s="44"/>
+      <c r="O7" s="44"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" s="30"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="37"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
+      <c r="N8" s="43"/>
+      <c r="O8" s="43"/>
+    </row>
+    <row r="9" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="30"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="4"/>
+    </row>
+    <row r="10" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="30"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="4"/>
+    </row>
+    <row r="11" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="30"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="4"/>
+    </row>
+    <row r="12" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="30"/>
+      <c r="B12" s="50"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="4"/>
+    </row>
+    <row r="13" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="30"/>
+      <c r="B13" s="50"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="4"/>
+    </row>
+    <row r="14" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="30"/>
+      <c r="B14" s="50"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="4"/>
+    </row>
+    <row r="15" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="47"/>
+      <c r="B15" s="50"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="16"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="4"/>
+    </row>
+    <row r="16" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C16" s="4"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="4"/>
+    </row>
+    <row r="17" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="4"/>
+    </row>
+    <row r="18" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="J18" s="4"/>
+    </row>
+    <row r="19" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="J19" s="4"/>
+      <c r="L19" s="43"/>
+      <c r="M19"/>
+    </row>
+    <row r="20" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="J20" s="4"/>
+    </row>
+    <row r="21" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="J21" s="4"/>
+    </row>
+    <row r="22" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="J22" s="4"/>
+    </row>
+    <row r="23" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="J23" s="4"/>
+    </row>
+    <row r="24" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="J24" s="4"/>
+    </row>
+    <row r="25" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C25" s="1"/>
+      <c r="E25" s="4"/>
+      <c r="J25" s="4"/>
+    </row>
+    <row r="26" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="B26" s="45" t="s">
+        <v>42</v>
+      </c>
+      <c r="C26" s="45" t="s">
+        <v>43</v>
+      </c>
+      <c r="E26" s="4"/>
+      <c r="J26" s="4"/>
+    </row>
+    <row r="27" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="30"/>
+      <c r="B27" s="11" t="s">
+        <v>420</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>419</v>
+      </c>
+      <c r="E27" s="4"/>
+      <c r="J27" s="4"/>
+    </row>
+    <row r="28" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="30"/>
+      <c r="B28" s="11" t="s">
+        <v>422</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>421</v>
+      </c>
+      <c r="E28" s="4"/>
+      <c r="J28" s="4"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29" s="30"/>
+      <c r="B29" s="11"/>
+      <c r="C29" s="11"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30" s="30"/>
+      <c r="B30" s="11"/>
+      <c r="C30" s="11"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A31" s="30"/>
+      <c r="B31" s="11"/>
+      <c r="C31" s="11"/>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A32" s="30"/>
+      <c r="B32" s="11"/>
+      <c r="C32" s="11"/>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A33" s="30"/>
+      <c r="B33" s="11"/>
+      <c r="C33" s="11"/>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K37" s="2"/>
+      <c r="L37" s="53" t="s">
+        <v>227</v>
+      </c>
+      <c r="M37" s="53" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K38" t="s">
+        <v>265</v>
+      </c>
+      <c r="L38" s="41" t="s">
+        <v>229</v>
+      </c>
+      <c r="M38" s="42" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K39" t="s">
+        <v>266</v>
+      </c>
+      <c r="L39" s="41" t="s">
+        <v>231</v>
+      </c>
+      <c r="M39" s="42" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C40" s="10"/>
+      <c r="K40" t="s">
+        <v>267</v>
+      </c>
+      <c r="L40" s="41" t="s">
+        <v>233</v>
+      </c>
+      <c r="M40" s="42" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C41" s="10"/>
+      <c r="K41" t="s">
+        <v>268</v>
+      </c>
+      <c r="L41" s="41" t="s">
+        <v>235</v>
+      </c>
+      <c r="M41" s="42" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C42" s="10"/>
+      <c r="K42" t="s">
+        <v>269</v>
+      </c>
+      <c r="L42" s="41" t="s">
+        <v>237</v>
+      </c>
+      <c r="M42" s="42" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K43" t="s">
+        <v>270</v>
+      </c>
+      <c r="L43" s="41" t="s">
+        <v>239</v>
+      </c>
+      <c r="M43" s="42" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K44" t="s">
+        <v>271</v>
+      </c>
+      <c r="L44" s="41" t="s">
+        <v>241</v>
+      </c>
+      <c r="M44" s="42" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K45" t="s">
+        <v>272</v>
+      </c>
+      <c r="L45" s="41" t="s">
+        <v>243</v>
+      </c>
+      <c r="M45" s="42" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K46" t="s">
+        <v>273</v>
+      </c>
+      <c r="L46" s="41" t="s">
+        <v>245</v>
+      </c>
+      <c r="M46" s="42" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K47" t="s">
+        <v>274</v>
+      </c>
+      <c r="L47" s="41" t="s">
+        <v>247</v>
+      </c>
+      <c r="M47" s="42" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K48" t="s">
+        <v>275</v>
+      </c>
+      <c r="L48" s="41" t="s">
+        <v>249</v>
+      </c>
+      <c r="M48" s="42" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="49" spans="11:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K49" t="s">
+        <v>276</v>
+      </c>
+      <c r="L49" s="41" t="s">
+        <v>251</v>
+      </c>
+      <c r="M49" s="42" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="50" spans="11:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K50" t="s">
+        <v>277</v>
+      </c>
+      <c r="L50" s="41" t="s">
+        <v>253</v>
+      </c>
+      <c r="M50" s="42" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="51" spans="11:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K51" t="s">
+        <v>278</v>
+      </c>
+      <c r="L51" s="41" t="s">
+        <v>255</v>
+      </c>
+      <c r="M51" s="42" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="52" spans="11:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K52" t="s">
+        <v>279</v>
+      </c>
+      <c r="L52" s="41" t="s">
+        <v>257</v>
+      </c>
+      <c r="M52" s="42" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="53" spans="11:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K53" t="s">
+        <v>280</v>
+      </c>
+      <c r="L53" s="41" t="s">
+        <v>259</v>
+      </c>
+      <c r="M53" s="52" t="s">
+        <v>438</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="M53" r:id="rId1" display="https://eur02.safelinks.protection.outlook.com/?url=https%3A%2F%2Fuat.mybeazleyus.com%2FBeazley%2FPolicy%2FPolicy%2FRecall%2F12756&amp;data=05%7C01%7CEmiliano.Duque%40beazley.com%7C1cd6041885234f8dd80508dad6e24cdc%7C9a50eba87568447abcb927a0d464aa80%7C0%7C0%7C638058564697769035%7CUnknown%7CTWFpbGZsb3d8eyJWIjoiMC4wLjAwMDAiLCJQIjoiV2luMzIiLCJBTiI6Ik1haWwiLCJXVCI6Mn0%3D%7C3000%7C%7C%7C&amp;sdata=8hGjJS5W2lysE7Goydkbjn0bQxZZWIa2JXJG1%2Ff02fM%3D&amp;reserved=0" xr:uid="{FF436DE4-4DFA-43A4-97D3-A2F7DC264A91}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0344D85-F638-4778-BEA4-92704756A748}">
   <dimension ref="A1:R57"/>
   <sheetViews>
@@ -8369,12 +9554,548 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD1398DB-13E2-474F-8F8D-D518D14A223D}">
+  <dimension ref="A1:Q53"/>
+  <sheetViews>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" style="4" customWidth="1"/>
+    <col min="3" max="3" width="103.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="1"/>
+    <col min="5" max="5" width="6.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="9.140625" style="1"/>
+    <col min="8" max="8" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" style="1"/>
+    <col min="10" max="10" width="9.140625" style="4"/>
+    <col min="11" max="11" width="9.140625" style="1"/>
+    <col min="12" max="12" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.140625" style="1"/>
+    <col min="16" max="16" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" s="23"/>
+      <c r="H1" s="4"/>
+    </row>
+    <row r="2" spans="1:17" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>187</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>384</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>200</v>
+      </c>
+      <c r="H2" s="15" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" s="30"/>
+      <c r="B3" s="11" t="s">
+        <v>402</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>401</v>
+      </c>
+      <c r="D3" s="16"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" s="30"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
+      <c r="N4" s="43"/>
+      <c r="O4" s="43"/>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="4"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" s="30"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="4"/>
+      <c r="Q5" s="4"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" s="30"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="49"/>
+      <c r="N6" s="44"/>
+      <c r="O6" s="44"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" s="30"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+      <c r="N7" s="44"/>
+      <c r="O7" s="44"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" s="30"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="37"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
+      <c r="N8" s="43"/>
+      <c r="O8" s="43"/>
+    </row>
+    <row r="9" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="30"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="4"/>
+    </row>
+    <row r="10" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="30"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="4"/>
+    </row>
+    <row r="11" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="30"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="4"/>
+    </row>
+    <row r="12" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="30"/>
+      <c r="B12" s="50"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="4"/>
+    </row>
+    <row r="13" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="30"/>
+      <c r="B13" s="50"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="4"/>
+    </row>
+    <row r="14" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="30"/>
+      <c r="B14" s="50"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="4"/>
+    </row>
+    <row r="15" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="47"/>
+      <c r="B15" s="50"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="16"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="4"/>
+    </row>
+    <row r="16" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C16" s="4"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="4"/>
+    </row>
+    <row r="17" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="4"/>
+    </row>
+    <row r="18" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="J18" s="4"/>
+    </row>
+    <row r="19" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="J19" s="4"/>
+      <c r="L19" s="43"/>
+      <c r="M19"/>
+    </row>
+    <row r="20" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="J20" s="4"/>
+    </row>
+    <row r="21" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="J21" s="4"/>
+    </row>
+    <row r="22" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="J22" s="4"/>
+    </row>
+    <row r="23" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="J23" s="4"/>
+    </row>
+    <row r="24" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="J24" s="4"/>
+    </row>
+    <row r="25" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C25" s="1"/>
+      <c r="E25" s="4"/>
+      <c r="J25" s="4"/>
+    </row>
+    <row r="26" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="B26" s="45" t="s">
+        <v>42</v>
+      </c>
+      <c r="C26" s="45" t="s">
+        <v>43</v>
+      </c>
+      <c r="E26" s="4"/>
+      <c r="J26" s="4"/>
+    </row>
+    <row r="27" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="30"/>
+      <c r="B27" s="11" t="s">
+        <v>402</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>401</v>
+      </c>
+      <c r="E27" s="4"/>
+      <c r="J27" s="4"/>
+    </row>
+    <row r="28" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="30"/>
+      <c r="B28" s="11"/>
+      <c r="C28" s="11"/>
+      <c r="E28" s="4"/>
+      <c r="J28" s="4"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29" s="30"/>
+      <c r="B29" s="11"/>
+      <c r="C29" s="11"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30" s="30"/>
+      <c r="B30" s="11"/>
+      <c r="C30" s="11"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A31" s="30"/>
+      <c r="B31" s="11"/>
+      <c r="C31" s="11"/>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A32" s="30"/>
+      <c r="B32" s="11"/>
+      <c r="C32" s="11"/>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A33" s="30"/>
+      <c r="B33" s="11"/>
+      <c r="C33" s="11"/>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K37" s="2"/>
+      <c r="L37" s="53" t="s">
+        <v>227</v>
+      </c>
+      <c r="M37" s="53" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K38" t="s">
+        <v>265</v>
+      </c>
+      <c r="L38" s="54" t="s">
+        <v>229</v>
+      </c>
+      <c r="M38" s="54" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K39" t="s">
+        <v>266</v>
+      </c>
+      <c r="L39" s="54" t="s">
+        <v>231</v>
+      </c>
+      <c r="M39" s="54" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C40" s="10"/>
+      <c r="K40" t="s">
+        <v>267</v>
+      </c>
+      <c r="L40" s="54" t="s">
+        <v>233</v>
+      </c>
+      <c r="M40" s="54" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C41" s="10"/>
+      <c r="K41" t="s">
+        <v>268</v>
+      </c>
+      <c r="L41" s="54" t="s">
+        <v>235</v>
+      </c>
+      <c r="M41" s="54" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C42" s="10"/>
+      <c r="K42" t="s">
+        <v>269</v>
+      </c>
+      <c r="L42" s="54" t="s">
+        <v>237</v>
+      </c>
+      <c r="M42" s="54" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K43" t="s">
+        <v>270</v>
+      </c>
+      <c r="L43" s="54" t="s">
+        <v>239</v>
+      </c>
+      <c r="M43" s="54" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K44" t="s">
+        <v>271</v>
+      </c>
+      <c r="L44" s="54" t="s">
+        <v>241</v>
+      </c>
+      <c r="M44" s="54" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K45" t="s">
+        <v>272</v>
+      </c>
+      <c r="L45" s="54" t="s">
+        <v>243</v>
+      </c>
+      <c r="M45" s="32" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K46" t="s">
+        <v>273</v>
+      </c>
+      <c r="L46" s="54" t="s">
+        <v>245</v>
+      </c>
+      <c r="M46" s="54" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K47" t="s">
+        <v>274</v>
+      </c>
+      <c r="L47" s="54" t="s">
+        <v>247</v>
+      </c>
+      <c r="M47" s="54" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K48" t="s">
+        <v>275</v>
+      </c>
+      <c r="L48" s="54" t="s">
+        <v>249</v>
+      </c>
+      <c r="M48" s="54" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="49" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="K49" t="s">
+        <v>276</v>
+      </c>
+      <c r="L49" s="54" t="s">
+        <v>251</v>
+      </c>
+      <c r="M49" s="54" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="50" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="K50" t="s">
+        <v>277</v>
+      </c>
+      <c r="L50" s="54" t="s">
+        <v>253</v>
+      </c>
+      <c r="M50" s="54" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="51" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="K51" t="s">
+        <v>278</v>
+      </c>
+      <c r="L51" s="54" t="s">
+        <v>255</v>
+      </c>
+      <c r="M51" s="54" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="52" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="K52" t="s">
+        <v>279</v>
+      </c>
+      <c r="L52" s="54" t="s">
+        <v>257</v>
+      </c>
+      <c r="M52" s="54" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="53" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="K53" t="s">
+        <v>280</v>
+      </c>
+      <c r="L53" s="54" t="s">
+        <v>259</v>
+      </c>
+      <c r="M53" s="54" t="s">
+        <v>418</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AA0CDE4-5F31-4494-98F0-8502D8AE5F10}">
   <dimension ref="A1:Q53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8753,7 +10474,9 @@
       <c r="J26" s="4"/>
     </row>
     <row r="27" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="30"/>
+      <c r="A27" s="30" t="s">
+        <v>4</v>
+      </c>
       <c r="B27" s="11" t="s">
         <v>371</v>
       </c>
@@ -8764,7 +10487,9 @@
       <c r="J27" s="4"/>
     </row>
     <row r="28" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="30"/>
+      <c r="A28" s="30" t="s">
+        <v>4</v>
+      </c>
       <c r="B28" s="11" t="s">
         <v>373</v>
       </c>
@@ -8775,7 +10500,9 @@
       <c r="J28" s="4"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A29" s="30"/>
+      <c r="A29" s="30" t="s">
+        <v>4</v>
+      </c>
       <c r="B29" s="11" t="s">
         <v>375</v>
       </c>
@@ -8784,7 +10511,9 @@
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A30" s="30"/>
+      <c r="A30" s="30" t="s">
+        <v>4</v>
+      </c>
       <c r="B30" s="11" t="s">
         <v>377</v>
       </c>
@@ -8793,7 +10522,9 @@
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A31" s="30"/>
+      <c r="A31" s="30" t="s">
+        <v>4</v>
+      </c>
       <c r="B31" s="11" t="s">
         <v>379</v>
       </c>
@@ -8802,7 +10533,9 @@
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A32" s="30"/>
+      <c r="A32" s="30" t="s">
+        <v>4</v>
+      </c>
       <c r="B32" s="11" t="s">
         <v>381</v>
       </c>
@@ -8810,8 +10543,19 @@
         <v>380</v>
       </c>
     </row>
-    <row r="36" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="37" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A33" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="B33" s="11" t="s">
+        <v>383</v>
+      </c>
+      <c r="C33" s="11" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="37" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K37" s="2"/>
       <c r="L37" s="39" t="s">
         <v>227</v>
@@ -8820,132 +10564,199 @@
         <v>228</v>
       </c>
     </row>
-    <row r="38" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K38" t="s">
         <v>265</v>
       </c>
-      <c r="L38" s="41"/>
-      <c r="M38" s="42"/>
-    </row>
-    <row r="39" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L38" s="41" t="s">
+        <v>229</v>
+      </c>
+      <c r="M38" s="42" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K39" t="s">
         <v>266</v>
       </c>
-      <c r="L39" s="41"/>
-      <c r="M39" s="42"/>
-    </row>
-    <row r="40" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L39" s="41" t="s">
+        <v>231</v>
+      </c>
+      <c r="M39" s="42" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C40" s="10"/>
       <c r="K40" t="s">
         <v>267</v>
       </c>
-      <c r="L40" s="41"/>
-      <c r="M40" s="42"/>
-    </row>
-    <row r="41" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L40" s="41" t="s">
+        <v>233</v>
+      </c>
+      <c r="M40" s="42" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C41" s="10"/>
       <c r="K41" t="s">
         <v>268</v>
       </c>
-      <c r="L41" s="41"/>
-      <c r="M41" s="42"/>
-    </row>
-    <row r="42" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L41" s="41" t="s">
+        <v>235</v>
+      </c>
+      <c r="M41" s="42" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C42" s="10"/>
       <c r="K42" t="s">
         <v>269</v>
       </c>
-      <c r="L42" s="41"/>
-      <c r="M42" s="42"/>
-    </row>
-    <row r="43" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L42" s="41" t="s">
+        <v>237</v>
+      </c>
+      <c r="M42" s="42" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K43" t="s">
         <v>270</v>
       </c>
-      <c r="L43" s="41"/>
-      <c r="M43" s="42"/>
-    </row>
-    <row r="44" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L43" s="41" t="s">
+        <v>239</v>
+      </c>
+      <c r="M43" s="42" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K44" t="s">
         <v>271</v>
       </c>
-      <c r="L44" s="41"/>
-      <c r="M44" s="42"/>
-    </row>
-    <row r="45" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L44" s="41" t="s">
+        <v>241</v>
+      </c>
+      <c r="M44" s="42" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K45" t="s">
         <v>272</v>
       </c>
-      <c r="L45" s="41"/>
-      <c r="M45" s="42"/>
-    </row>
-    <row r="46" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L45" s="41" t="s">
+        <v>243</v>
+      </c>
+      <c r="M45" s="42" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K46" t="s">
         <v>273</v>
       </c>
-      <c r="L46" s="41"/>
-      <c r="M46" s="42"/>
-    </row>
-    <row r="47" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L46" s="41" t="s">
+        <v>245</v>
+      </c>
+      <c r="M46" s="42" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K47" t="s">
         <v>274</v>
       </c>
-      <c r="L47" s="41"/>
-      <c r="M47" s="42"/>
-    </row>
-    <row r="48" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L47" s="41" t="s">
+        <v>247</v>
+      </c>
+      <c r="M47" s="42" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K48" t="s">
         <v>275</v>
       </c>
-      <c r="L48" s="41"/>
-      <c r="M48" s="42"/>
+      <c r="L48" s="41" t="s">
+        <v>249</v>
+      </c>
+      <c r="M48" s="42" t="s">
+        <v>395</v>
+      </c>
     </row>
     <row r="49" spans="11:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K49" t="s">
         <v>276</v>
       </c>
-      <c r="L49" s="41"/>
-      <c r="M49" s="42"/>
+      <c r="L49" s="41" t="s">
+        <v>251</v>
+      </c>
+      <c r="M49" s="42" t="s">
+        <v>396</v>
+      </c>
     </row>
     <row r="50" spans="11:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K50" t="s">
         <v>277</v>
       </c>
-      <c r="L50" s="41"/>
-      <c r="M50" s="42"/>
+      <c r="L50" s="41" t="s">
+        <v>253</v>
+      </c>
+      <c r="M50" s="42" t="s">
+        <v>397</v>
+      </c>
     </row>
     <row r="51" spans="11:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K51" t="s">
         <v>278</v>
       </c>
-      <c r="L51" s="41"/>
-      <c r="M51" s="42"/>
+      <c r="L51" s="41" t="s">
+        <v>255</v>
+      </c>
+      <c r="M51" s="42" t="s">
+        <v>398</v>
+      </c>
     </row>
     <row r="52" spans="11:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K52" t="s">
         <v>279</v>
       </c>
-      <c r="L52" s="41"/>
-      <c r="M52" s="51"/>
+      <c r="L52" s="41" t="s">
+        <v>257</v>
+      </c>
+      <c r="M52" s="52" t="s">
+        <v>399</v>
+      </c>
     </row>
     <row r="53" spans="11:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K53" t="s">
         <v>280</v>
       </c>
-      <c r="L53" s="41"/>
-      <c r="M53" s="42"/>
+      <c r="L53" s="41" t="s">
+        <v>259</v>
+      </c>
+      <c r="M53" s="42" t="s">
+        <v>400</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="M52" r:id="rId1" display="https://eur02.safelinks.protection.outlook.com/?url=https%3A%2F%2Fuat.mybeazleyus.com%2FBeazley%2FPolicy%2FPolicy%2FRecall%2F12646&amp;data=05%7C01%7CEmiliano.Duque%40beazley.com%7Cc99f63693e2a4abc136908dacd658516%7C9a50eba87568447abcb927a0d464aa80%7C0%7C0%7C638048133145002998%7CUnknown%7CTWFpbGZsb3d8eyJWIjoiMC4wLjAwMDAiLCJQIjoiV2luMzIiLCJBTiI6Ik1haWwiLCJXVCI6Mn0%3D%7C3000%7C%7C%7C&amp;sdata=xfzFS%2F0QA4Yi1WIcPYSAiKFJfc9OI5P9cS4dsi8u%2BEQ%3D&amp;reserved=0" xr:uid="{551789AB-6F9A-42AE-A018-1A7D95110F69}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AED93280-0C8D-4F07-8DF1-98873AFA4F7A}">
   <dimension ref="A1:Q53"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="A26" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="C64" sqref="C64"/>
     </sheetView>
   </sheetViews>
@@ -9685,11 +11496,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{388FBC72-9C75-4760-AE51-A2960690EEEA}">
   <dimension ref="A1:Q41"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="A33" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="C74" sqref="C74"/>
     </sheetView>
   </sheetViews>
@@ -10146,7 +11957,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{825A66BC-B9F8-4493-904A-635C22EE8433}">
   <dimension ref="A1:Q28"/>
   <sheetViews>
@@ -10578,7 +12389,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{823E4EE9-9C9A-417F-96ED-A88DDB9D56A7}">
   <dimension ref="A1:Q28"/>
   <sheetViews>
@@ -11048,7 +12859,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBAA9453-34AC-469C-B066-9F9AA2A7731A}">
   <dimension ref="A1:Q30"/>
   <sheetViews>
@@ -11549,439 +13360,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34226C2A-68CD-4BD9-A906-AC8705245632}">
-  <dimension ref="A1:E4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" customWidth="1"/>
-    <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="s">
-        <v>188</v>
-      </c>
-      <c r="B1" s="34" t="s">
-        <v>189</v>
-      </c>
-      <c r="C1" s="34" t="s">
-        <v>190</v>
-      </c>
-      <c r="D1" s="34" t="s">
-        <v>191</v>
-      </c>
-      <c r="E1" s="34" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="32" t="s">
-        <v>218</v>
-      </c>
-      <c r="B2" s="32">
-        <v>1</v>
-      </c>
-      <c r="C2" s="32">
-        <v>6</v>
-      </c>
-      <c r="D2" s="32">
-        <v>0</v>
-      </c>
-      <c r="E2" s="32" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="32" t="s">
-        <v>220</v>
-      </c>
-      <c r="B3" s="32">
-        <v>1</v>
-      </c>
-      <c r="C3" s="32">
-        <v>2</v>
-      </c>
-      <c r="D3" s="32">
-        <v>0</v>
-      </c>
-      <c r="E3" s="32" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="32" t="s">
-        <v>222</v>
-      </c>
-      <c r="B4" s="32">
-        <v>1</v>
-      </c>
-      <c r="C4" s="32">
-        <v>2</v>
-      </c>
-      <c r="D4" s="32">
-        <v>0</v>
-      </c>
-      <c r="E4" s="32" t="s">
-        <v>223</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E786991-4988-4254-B35C-AD773FF122DA}">
-  <dimension ref="A1:R39"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" style="4" customWidth="1"/>
-    <col min="3" max="3" width="132.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="1"/>
-    <col min="5" max="5" width="6.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="9.140625" style="1"/>
-    <col min="8" max="8" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" style="1"/>
-    <col min="10" max="10" width="9.140625" style="4"/>
-    <col min="11" max="15" width="9.140625" style="1"/>
-    <col min="16" max="16" width="51.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.140625" style="1"/>
-    <col min="19" max="19" width="22.42578125" style="1" customWidth="1"/>
-    <col min="20" max="16384" width="9.140625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" s="23"/>
-      <c r="H1" s="4"/>
-    </row>
-    <row r="2" spans="1:18" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>103</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="D2" s="15" t="s">
-        <v>187</v>
-      </c>
-      <c r="E2" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="F2" s="15" t="s">
-        <v>149</v>
-      </c>
-      <c r="G2" s="15" t="s">
-        <v>151</v>
-      </c>
-      <c r="H2" s="15" t="s">
-        <v>200</v>
-      </c>
-      <c r="I2" s="15" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="30"/>
-      <c r="B3" s="11" t="s">
-        <v>206</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>205</v>
-      </c>
-      <c r="D3" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" s="37" t="s">
-        <v>217</v>
-      </c>
-      <c r="F3" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="30"/>
-      <c r="B4" s="11" t="s">
-        <v>215</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>216</v>
-      </c>
-      <c r="D4" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="E4" s="37" t="s">
-        <v>217</v>
-      </c>
-      <c r="F4" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="16"/>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" s="36"/>
-      <c r="B5" s="28"/>
-      <c r="C5" s="28"/>
-      <c r="D5" s="35"/>
-      <c r="E5" s="36"/>
-      <c r="F5" s="35"/>
-      <c r="G5" s="35"/>
-      <c r="H5" s="35"/>
-      <c r="I5" s="35"/>
-      <c r="O5" s="4"/>
-      <c r="P5" s="4"/>
-      <c r="Q5" s="4"/>
-      <c r="R5" s="4"/>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6" s="36"/>
-      <c r="B6" s="28"/>
-      <c r="C6" s="28"/>
-      <c r="D6" s="35"/>
-      <c r="E6" s="36"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="35"/>
-      <c r="H6" s="35"/>
-      <c r="I6" s="35"/>
-      <c r="O6" s="4"/>
-      <c r="P6" s="4"/>
-      <c r="Q6" s="4"/>
-      <c r="R6" s="4"/>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-    </row>
-    <row r="11" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="J11" s="4"/>
-    </row>
-    <row r="12" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="J12" s="4"/>
-    </row>
-    <row r="13" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="J13" s="4"/>
-    </row>
-    <row r="14" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="B14" s="5"/>
-      <c r="C14" s="21"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="J14" s="4"/>
-    </row>
-    <row r="15" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="J15" s="4"/>
-    </row>
-    <row r="16" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="J16" s="4"/>
-    </row>
-    <row r="17" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="J17" s="4"/>
-    </row>
-    <row r="18" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="J18" s="4"/>
-    </row>
-    <row r="19" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="J19" s="4"/>
-    </row>
-    <row r="20" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="J20" s="4"/>
-    </row>
-    <row r="21" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="B21" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="C21" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="D21" s="1"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="J21" s="4"/>
-    </row>
-    <row r="22" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="30"/>
-      <c r="B22" s="11" t="s">
-        <v>206</v>
-      </c>
-      <c r="C22" s="11" t="s">
-        <v>205</v>
-      </c>
-      <c r="D22" s="1"/>
-      <c r="E22" s="4"/>
-      <c r="J22" s="4"/>
-    </row>
-    <row r="23" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="30"/>
-      <c r="B23" s="11" t="s">
-        <v>215</v>
-      </c>
-      <c r="C23" s="11" t="s">
-        <v>216</v>
-      </c>
-      <c r="E23" s="4"/>
-      <c r="J23" s="4"/>
-    </row>
-    <row r="24" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="J24" s="4"/>
-    </row>
-    <row r="25" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="J25" s="4"/>
-    </row>
-    <row r="26" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="4"/>
-      <c r="E26" s="4"/>
-      <c r="J26" s="4"/>
-    </row>
-    <row r="27" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="J27" s="4"/>
-    </row>
-    <row r="28" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="J28" s="4"/>
-    </row>
-    <row r="29" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="4"/>
-      <c r="E29" s="4"/>
-      <c r="J29" s="4"/>
-    </row>
-    <row r="30" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="4"/>
-      <c r="E30" s="4"/>
-      <c r="J30" s="4"/>
-    </row>
-    <row r="31" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="4"/>
-      <c r="E31" s="4"/>
-      <c r="J31" s="4"/>
-    </row>
-    <row r="32" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="4"/>
-      <c r="E32" s="4"/>
-      <c r="J32" s="4"/>
-    </row>
-    <row r="33" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="4"/>
-      <c r="E33" s="4"/>
-      <c r="J33" s="4"/>
-    </row>
-    <row r="34" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="4"/>
-      <c r="E34" s="4"/>
-      <c r="J34" s="4"/>
-    </row>
-    <row r="35" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="4"/>
-      <c r="E35" s="4"/>
-      <c r="J35" s="4"/>
-    </row>
-    <row r="36" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="4"/>
-      <c r="E36" s="4"/>
-      <c r="J36" s="4"/>
-    </row>
-    <row r="37" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="4"/>
-      <c r="E37" s="4"/>
-      <c r="J37" s="4"/>
-    </row>
-    <row r="38" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="4"/>
-      <c r="E38" s="4"/>
-      <c r="J38" s="4"/>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" s="3"/>
-      <c r="C39" s="3"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>